<commit_message>
excel to json file
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kim/Downloads/parcel-static-html/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A5B0D2-268A-AB40-B536-5C89969C3EC0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342F38BB-2549-8441-B9A6-5E221DDB59FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{710D6B70-2B13-8446-BE2B-45DD5E17E75F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>dragon</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -69,6 +69,18 @@
   </si>
   <si>
     <t>dragon sea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bdo_kr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bdo_en</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>country</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -433,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93AADA16-CC1C-2642-B0D1-6876D2C24751}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -446,36 +458,45 @@
     <col min="3" max="3" width="55.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>